<commit_message>
estimated pulp time complexity with curve fitting and made first draft of ranking algorithms based on their performance, specifically gurobi vs 2nd heuristic algo
</commit_message>
<xml_diff>
--- a/src/in/Data assignment parcel transport 2 TEST.xlsx
+++ b/src/in/Data assignment parcel transport 2 TEST.xlsx
@@ -66,7 +66,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -76,6 +76,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1911,44 +1917,24 @@
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="B11" s="1">
-        <v>20908.0</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="B12" s="1">
-        <v>27858.0</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="B13" s="1">
-        <v>24488.0</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="B14" s="1">
-        <v>32660.0</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="B15" s="1">
-        <v>26253.0</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="1"/>
@@ -3152,21 +3138,11 @@
       <c r="K1" s="1">
         <v>10.0</v>
       </c>
-      <c r="L1" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="M1" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="N1" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="O1" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="P1" s="1">
-        <v>15.0</v>
-      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -3217,51 +3193,41 @@
       <c r="A2" s="1">
         <v>1.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="5">
         <v>0.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="5">
+        <v>15.0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>39.0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>33.0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>27.0</v>
+      </c>
+      <c r="H2" s="5">
         <v>20.0</v>
       </c>
-      <c r="D2" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="I2" s="5">
+        <v>18.0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="K2" s="5">
         <v>23.0</v>
       </c>
-      <c r="F2" s="1">
-        <v>23.0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>33.0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="M2" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="O2" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="P2" s="1">
-        <v>13.0</v>
-      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -3312,51 +3278,41 @@
       <c r="A3" s="1">
         <v>2.0</v>
       </c>
-      <c r="B3" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="5">
+        <v>15.0</v>
+      </c>
+      <c r="C3" s="5">
         <v>0.0</v>
       </c>
-      <c r="D3" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="D3" s="5">
+        <v>37.0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>23.0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="I3" s="5">
         <v>13.0</v>
       </c>
-      <c r="F3" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>38.0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>22.0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>27.0</v>
-      </c>
-      <c r="O3" s="1">
+      <c r="J3" s="5">
+        <v>34.0</v>
+      </c>
+      <c r="K3" s="5">
         <v>35.0</v>
       </c>
-      <c r="P3" s="1">
-        <v>20.0</v>
-      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -3407,51 +3363,41 @@
       <c r="A4" s="1">
         <v>3.0</v>
       </c>
-      <c r="B4" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="B4" s="5">
+        <v>39.0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>37.0</v>
+      </c>
+      <c r="D4" s="5">
         <v>0.0</v>
       </c>
-      <c r="E4" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="E4" s="5">
+        <v>31.0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>21.0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>22.0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>34.0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>35.0</v>
+      </c>
+      <c r="K4" s="5">
         <v>7.0</v>
       </c>
-      <c r="G4" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>21.0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>21.0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="M4" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="O4" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="P4" s="1">
-        <v>23.0</v>
-      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -3502,51 +3448,41 @@
       <c r="A5" s="1">
         <v>4.0</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>31.0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>28.0</v>
+      </c>
+      <c r="G5" s="5">
         <v>23.0</v>
       </c>
-      <c r="C5" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>27.0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="L5" s="1">
+      <c r="H5" s="5">
+        <v>33.0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>39.0</v>
+      </c>
+      <c r="K5" s="5">
         <v>8.0</v>
       </c>
-      <c r="M5" s="1">
-        <v>33.0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>35.0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>16.0</v>
-      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -3597,51 +3533,41 @@
       <c r="A6" s="1">
         <v>5.0</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
+        <v>33.0</v>
+      </c>
+      <c r="C6" s="5">
         <v>23.0</v>
       </c>
-      <c r="C6" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="D6" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>28.0</v>
+      </c>
+      <c r="F6" s="5">
         <v>0.0</v>
       </c>
-      <c r="G6" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="K6" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="L6" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="M6" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="N6" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="O6" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="P6" s="1">
-        <v>15.0</v>
-      </c>
+      <c r="G6" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>26.0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>33.0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>33.0</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -3692,51 +3618,41 @@
       <c r="A7" s="1">
         <v>6.0</v>
       </c>
-      <c r="B7" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="B7" s="5">
+        <v>27.0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>21.0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>23.0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="G7" s="5">
         <v>0.0</v>
       </c>
-      <c r="H7" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="K7" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="L7" s="1">
-        <v>29.0</v>
-      </c>
-      <c r="M7" s="1">
-        <v>21.0</v>
-      </c>
-      <c r="N7" s="1">
-        <v>29.0</v>
-      </c>
-      <c r="O7" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="P7" s="1">
-        <v>16.0</v>
-      </c>
+      <c r="H7" s="5">
+        <v>22.0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>35.0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>23.0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>31.0</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -3787,51 +3703,41 @@
       <c r="A8" s="1">
         <v>7.0</v>
       </c>
-      <c r="B8" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="B8" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>22.0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>33.0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>22.0</v>
+      </c>
+      <c r="H8" s="5">
         <v>0.0</v>
       </c>
-      <c r="I8" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="L8" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="M8" s="1">
-        <v>29.0</v>
-      </c>
-      <c r="N8" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="O8" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="P8" s="1">
-        <v>34.0</v>
-      </c>
+      <c r="I8" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>12.0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -3882,51 +3788,41 @@
       <c r="A9" s="1">
         <v>8.0</v>
       </c>
-      <c r="B9" s="1">
-        <v>33.0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="B9" s="5">
         <v>18.0</v>
       </c>
-      <c r="E9" s="1">
+      <c r="C9" s="5">
         <v>13.0</v>
       </c>
-      <c r="F9" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="D9" s="5">
+        <v>34.0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>26.0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>35.0</v>
+      </c>
+      <c r="H9" s="5">
         <v>8.0</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>14.0</v>
+      </c>
+      <c r="K9" s="5">
         <v>9.0</v>
       </c>
-      <c r="I9" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="K9" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="L9" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="M9" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="N9" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="O9" s="1">
-        <v>35.0</v>
-      </c>
-      <c r="P9" s="1">
-        <v>33.0</v>
-      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -3977,51 +3873,41 @@
       <c r="A10" s="1">
         <v>9.0</v>
       </c>
-      <c r="B10" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>38.0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>21.0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>27.0</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="B10" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>34.0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>35.0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>39.0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>33.0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>23.0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>12.0</v>
+      </c>
+      <c r="I10" s="5">
         <v>14.0</v>
       </c>
-      <c r="G10" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="J10" s="1">
+      <c r="J10" s="5">
         <v>0.0</v>
       </c>
-      <c r="K10" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="L10" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="M10" s="1">
-        <v>29.0</v>
-      </c>
-      <c r="N10" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="O10" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="P10" s="1">
-        <v>20.0</v>
-      </c>
+      <c r="K10" s="5">
+        <v>19.0</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -4072,51 +3958,41 @@
       <c r="A11" s="1">
         <v>10.0</v>
       </c>
-      <c r="B11" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B11" s="5">
+        <v>23.0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>35.0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>33.0</v>
+      </c>
+      <c r="G11" s="5">
         <v>31.0</v>
       </c>
-      <c r="D11" s="1">
-        <v>21.0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="K11" s="1">
+      <c r="H11" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>19.0</v>
+      </c>
+      <c r="K11" s="5">
         <v>0.0</v>
       </c>
-      <c r="L11" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="M11" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="N11" s="1">
-        <v>29.0</v>
-      </c>
-      <c r="O11" s="1">
-        <v>28.0</v>
-      </c>
-      <c r="P11" s="1">
-        <v>7.0</v>
-      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -4164,54 +4040,22 @@
       <c r="BI11" s="1"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="B12" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>29.0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="L12" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="M12" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="N12" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="O12" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="P12" s="1">
-        <v>15.0</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -4259,54 +4103,22 @@
       <c r="BI12" s="1"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="B13" s="3">
-        <v>24.0</v>
-      </c>
-      <c r="C13" s="3">
-        <v>22.0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>20.0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>33.0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>17.0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>21.0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>29.0</v>
-      </c>
-      <c r="I13" s="3">
-        <v>30.0</v>
-      </c>
-      <c r="J13" s="3">
-        <v>29.0</v>
-      </c>
-      <c r="K13" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="L13" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="M13" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="N13" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="O13" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="P13" s="1">
-        <v>35.0</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -4354,54 +4166,22 @@
       <c r="BI13" s="1"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="B14" s="3">
-        <v>11.0</v>
-      </c>
-      <c r="C14" s="3">
-        <v>27.0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>30.0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>9.0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>31.0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>29.0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>17.0</v>
-      </c>
-      <c r="I14" s="3">
-        <v>19.0</v>
-      </c>
-      <c r="J14" s="3">
-        <v>6.0</v>
-      </c>
-      <c r="K14" s="3">
-        <v>29.0</v>
-      </c>
-      <c r="L14" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="M14" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="O14" s="1">
-        <v>33.0</v>
-      </c>
-      <c r="P14" s="1">
-        <v>10.0</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -4449,54 +4229,22 @@
       <c r="BI14" s="1"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="B15" s="3">
-        <v>24.0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>35.0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>13.0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>35.0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>13.0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>10.0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>26.0</v>
-      </c>
-      <c r="I15" s="3">
-        <v>35.0</v>
-      </c>
-      <c r="J15" s="3">
-        <v>16.0</v>
-      </c>
-      <c r="K15" s="3">
-        <v>28.0</v>
-      </c>
-      <c r="L15" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="M15" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="N15" s="1">
-        <v>33.0</v>
-      </c>
-      <c r="O15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="P15" s="1">
-        <v>29.0</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -4544,54 +4292,22 @@
       <c r="BI15" s="1"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="B16" s="3">
-        <v>13.0</v>
-      </c>
-      <c r="C16" s="3">
-        <v>20.0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>16.0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>15.0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>16.0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>34.0</v>
-      </c>
-      <c r="I16" s="3">
-        <v>33.0</v>
-      </c>
-      <c r="J16" s="3">
-        <v>20.0</v>
-      </c>
-      <c r="K16" s="3">
-        <v>7.0</v>
-      </c>
-      <c r="L16" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="M16" s="1">
-        <v>35.0</v>
-      </c>
-      <c r="N16" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="O16" s="1">
-        <v>29.0</v>
-      </c>
-      <c r="P16" s="1">
-        <v>0.0</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -9228,21 +8944,11 @@
       <c r="K1" s="1">
         <v>10.0</v>
       </c>
-      <c r="L1" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="M1" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="N1" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="O1" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="P1" s="1">
-        <v>15.0</v>
-      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -9293,51 +8999,41 @@
       <c r="A2" s="1">
         <v>1.0</v>
       </c>
-      <c r="B2" s="3">
-        <v>75.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>37.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>55.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>19.0</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="B2" s="6">
+        <v>42.0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>23.0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>58.0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>46.0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>26.0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>32.0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>30.0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>58.0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>28.0</v>
+      </c>
+      <c r="K2" s="6">
         <v>20.0</v>
       </c>
-      <c r="G2" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>57.0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>17.0</v>
-      </c>
-      <c r="J2" s="3">
-        <v>19.0</v>
-      </c>
-      <c r="K2" s="3">
-        <v>16.0</v>
-      </c>
-      <c r="L2" s="3">
-        <v>308.0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>31.0</v>
-      </c>
-      <c r="N2" s="3">
-        <v>278.0</v>
-      </c>
-      <c r="O2" s="3">
-        <v>154.0</v>
-      </c>
-      <c r="P2" s="3">
-        <v>33.0</v>
-      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
@@ -9388,51 +9084,41 @@
       <c r="A3" s="1">
         <v>2.0</v>
       </c>
-      <c r="B3" s="3">
-        <v>26.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>38.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>25.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>27.0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="B3" s="6">
+        <v>47.0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>144.0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>35.0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>44.0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>66.0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>29.0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>44.0</v>
+      </c>
+      <c r="I3" s="6">
         <v>23.0</v>
       </c>
-      <c r="H3" s="3">
-        <v>38.0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>20.0</v>
-      </c>
-      <c r="J3" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="K3" s="3">
-        <v>17.0</v>
-      </c>
-      <c r="L3" s="3">
-        <v>253.0</v>
-      </c>
-      <c r="M3" s="3">
-        <v>127.0</v>
-      </c>
-      <c r="N3" s="3">
-        <v>318.0</v>
-      </c>
-      <c r="O3" s="3">
-        <v>48.0</v>
-      </c>
-      <c r="P3" s="3">
-        <v>118.0</v>
-      </c>
+      <c r="J3" s="6">
+        <v>56.0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>32.0</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
@@ -9483,51 +9169,41 @@
       <c r="A4" s="1">
         <v>3.0</v>
       </c>
-      <c r="B4" s="3">
-        <v>67.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>39.0</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="B4" s="6">
+        <v>14.0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>42.0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>29.0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>27.0</v>
+      </c>
+      <c r="F4" s="6">
         <v>51.0</v>
       </c>
-      <c r="E4" s="3">
-        <v>22.0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>24.0</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="G4" s="6">
+        <v>25.0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>49.0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>19.0</v>
+      </c>
+      <c r="J4" s="6">
         <v>21.0</v>
       </c>
-      <c r="H4" s="3">
-        <v>71.0</v>
-      </c>
-      <c r="I4" s="3">
-        <v>20.0</v>
-      </c>
-      <c r="J4" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="K4" s="3">
-        <v>19.0</v>
-      </c>
-      <c r="L4" s="3">
-        <v>118.0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>211.0</v>
-      </c>
-      <c r="N4" s="3">
-        <v>31.0</v>
-      </c>
-      <c r="O4" s="3">
-        <v>287.0</v>
-      </c>
-      <c r="P4" s="3">
-        <v>233.0</v>
-      </c>
+      <c r="K4" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
@@ -9578,51 +9254,41 @@
       <c r="A5" s="1">
         <v>4.0</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="6">
+        <v>31.0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>42.0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>61.0</v>
+      </c>
+      <c r="E5" s="6">
         <v>17.0</v>
       </c>
-      <c r="C5" s="3">
-        <v>33.0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>19.0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>25.0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>16.0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>40.0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="F5" s="6">
+        <v>165.0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>17.0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>37.0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>42.0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>21.0</v>
+      </c>
+      <c r="K5" s="6">
         <v>11.0</v>
       </c>
-      <c r="K5" s="3">
-        <v>19.0</v>
-      </c>
-      <c r="L5" s="3">
-        <v>139.0</v>
-      </c>
-      <c r="M5" s="3">
-        <v>255.0</v>
-      </c>
-      <c r="N5" s="3">
-        <v>229.0</v>
-      </c>
-      <c r="O5" s="3">
-        <v>89.0</v>
-      </c>
-      <c r="P5" s="3">
-        <v>266.0</v>
-      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
@@ -9673,51 +9339,41 @@
       <c r="A6" s="1">
         <v>5.0</v>
       </c>
-      <c r="B6" s="3">
-        <v>17.0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>25.0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>21.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>19.0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>73.0</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="B6" s="6">
+        <v>30.0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>50.0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>12.0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>94.0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>69.0</v>
+      </c>
+      <c r="I6" s="6">
         <v>20.0</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="6">
         <v>24.0</v>
       </c>
-      <c r="K6" s="3">
-        <v>19.0</v>
-      </c>
-      <c r="L6" s="3">
-        <v>133.0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>82.0</v>
-      </c>
-      <c r="N6" s="3">
-        <v>72.0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>68.0</v>
-      </c>
-      <c r="P6" s="3">
-        <v>236.0</v>
-      </c>
+      <c r="K6" s="6">
+        <v>28.0</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
@@ -9768,51 +9424,41 @@
       <c r="A7" s="1">
         <v>6.0</v>
       </c>
-      <c r="B7" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="B7" s="6">
+        <v>38.0</v>
+      </c>
+      <c r="C7" s="6">
+        <v>23.0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>67.0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>23.0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>40.0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>30.0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>58.0</v>
+      </c>
+      <c r="I7" s="6">
         <v>16.0</v>
       </c>
-      <c r="F7" s="3">
-        <v>11.0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>17.0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>37.0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>22.0</v>
-      </c>
-      <c r="J7" s="3">
-        <v>10.0</v>
-      </c>
-      <c r="K7" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="L7" s="3">
-        <v>65.0</v>
-      </c>
-      <c r="M7" s="3">
-        <v>44.0</v>
-      </c>
-      <c r="N7" s="3">
-        <v>257.0</v>
-      </c>
-      <c r="O7" s="3">
-        <v>58.0</v>
-      </c>
-      <c r="P7" s="3">
-        <v>176.0</v>
-      </c>
+      <c r="J7" s="6">
+        <v>63.0</v>
+      </c>
+      <c r="K7" s="6">
+        <v>13.0</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
@@ -9863,51 +9509,41 @@
       <c r="A8" s="1">
         <v>7.0</v>
       </c>
-      <c r="B8" s="3">
-        <v>82.0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>78.0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>90.0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>68.0</v>
-      </c>
-      <c r="F8" s="3">
-        <v>95.0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>73.0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>312.0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>99.0</v>
-      </c>
-      <c r="J8" s="3">
-        <v>110.0</v>
-      </c>
-      <c r="K8" s="3">
-        <v>110.0</v>
-      </c>
-      <c r="L8" s="3">
-        <v>308.0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>52.0</v>
-      </c>
-      <c r="N8" s="3">
-        <v>77.0</v>
-      </c>
-      <c r="O8" s="3">
-        <v>217.0</v>
-      </c>
-      <c r="P8" s="3">
-        <v>102.0</v>
-      </c>
+      <c r="B8" s="6">
+        <v>98.0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>94.0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>12.0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>56.0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>128.0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>40.0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>66.0</v>
+      </c>
+      <c r="I8" s="6">
+        <v>11.0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>49.0</v>
+      </c>
+      <c r="K8" s="6">
+        <v>21.0</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
@@ -9958,51 +9594,41 @@
       <c r="A9" s="1">
         <v>8.0</v>
       </c>
-      <c r="B9" s="3">
-        <v>35.0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>42.0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>36.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>48.0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>36.0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>58.0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>173.0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>90.0</v>
-      </c>
-      <c r="J9" s="3">
-        <v>41.0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>92.0</v>
-      </c>
-      <c r="L9" s="3">
-        <v>315.0</v>
-      </c>
-      <c r="M9" s="3">
-        <v>299.0</v>
-      </c>
-      <c r="N9" s="3">
-        <v>191.0</v>
-      </c>
-      <c r="O9" s="3">
-        <v>37.0</v>
-      </c>
-      <c r="P9" s="3">
-        <v>270.0</v>
-      </c>
+      <c r="B9" s="6">
+        <v>34.0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>12.0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>20.0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>45.0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>17.0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>70.0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>64.0</v>
+      </c>
+      <c r="I9" s="6">
+        <v>31.0</v>
+      </c>
+      <c r="J9" s="6">
+        <v>18.0</v>
+      </c>
+      <c r="K9" s="6">
+        <v>18.0</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -10053,51 +9679,41 @@
       <c r="A10" s="1">
         <v>9.0</v>
       </c>
-      <c r="B10" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>15.0</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="B10" s="6">
+        <v>35.0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>17.0</v>
+      </c>
+      <c r="D10" s="6">
         <v>10.0</v>
       </c>
-      <c r="F10" s="3">
-        <v>19.0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>11.0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>68.0</v>
-      </c>
-      <c r="I10" s="3">
-        <v>15.0</v>
-      </c>
-      <c r="J10" s="3">
-        <v>24.0</v>
-      </c>
-      <c r="K10" s="3">
-        <v>20.0</v>
-      </c>
-      <c r="L10" s="3">
-        <v>168.0</v>
-      </c>
-      <c r="M10" s="3">
-        <v>47.0</v>
-      </c>
-      <c r="N10" s="3">
-        <v>210.0</v>
-      </c>
-      <c r="O10" s="3">
-        <v>55.0</v>
-      </c>
-      <c r="P10" s="3">
-        <v>50.0</v>
-      </c>
+      <c r="E10" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>33.0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>25.0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>16.0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>87.0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>37.0</v>
+      </c>
+      <c r="K10" s="6">
+        <v>43.0</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
@@ -10148,51 +9764,41 @@
       <c r="A11" s="1">
         <v>10.0</v>
       </c>
-      <c r="B11" s="3">
-        <v>22.0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>25.0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="B11" s="6">
+        <v>34.0</v>
+      </c>
+      <c r="C11" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>60.0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>45.0</v>
+      </c>
+      <c r="F11" s="6">
         <v>28.0</v>
       </c>
-      <c r="F11" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>33.0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>109.0</v>
-      </c>
-      <c r="I11" s="3">
-        <v>51.0</v>
-      </c>
-      <c r="J11" s="3">
-        <v>30.0</v>
-      </c>
-      <c r="K11" s="3">
-        <v>63.0</v>
-      </c>
-      <c r="L11" s="3">
-        <v>190.0</v>
-      </c>
-      <c r="M11" s="3">
-        <v>319.0</v>
-      </c>
-      <c r="N11" s="3">
-        <v>186.0</v>
-      </c>
-      <c r="O11" s="3">
-        <v>29.0</v>
-      </c>
-      <c r="P11" s="3">
-        <v>200.0</v>
-      </c>
+      <c r="G11" s="6">
+        <v>46.0</v>
+      </c>
+      <c r="H11" s="6">
+        <v>13.0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="K11" s="6">
+        <v>28.0</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
@@ -10240,54 +9846,22 @@
       <c r="BI11" s="3"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="B12" s="3">
-        <v>14.0</v>
-      </c>
-      <c r="C12" s="3">
-        <v>105.0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>267.0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>246.0</v>
-      </c>
-      <c r="F12" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>269.0</v>
-      </c>
-      <c r="H12" s="3">
-        <v>131.0</v>
-      </c>
-      <c r="I12" s="3">
-        <v>229.0</v>
-      </c>
-      <c r="J12" s="3">
-        <v>253.0</v>
-      </c>
-      <c r="K12" s="3">
-        <v>269.0</v>
-      </c>
-      <c r="L12" s="3">
-        <v>89.0</v>
-      </c>
-      <c r="M12" s="3">
-        <v>224.0</v>
-      </c>
-      <c r="N12" s="3">
-        <v>144.0</v>
-      </c>
-      <c r="O12" s="3">
-        <v>123.0</v>
-      </c>
-      <c r="P12" s="3">
-        <v>305.0</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
@@ -10335,54 +9909,22 @@
       <c r="BI12" s="3"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="B13" s="3">
-        <v>245.0</v>
-      </c>
-      <c r="C13" s="3">
-        <v>274.0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>306.0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>13.0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>227.0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>131.0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>57.0</v>
-      </c>
-      <c r="I13" s="3">
-        <v>256.0</v>
-      </c>
-      <c r="J13" s="3">
-        <v>65.0</v>
-      </c>
-      <c r="K13" s="3">
-        <v>196.0</v>
-      </c>
-      <c r="L13" s="3">
-        <v>310.0</v>
-      </c>
-      <c r="M13" s="3">
-        <v>203.0</v>
-      </c>
-      <c r="N13" s="3">
-        <v>48.0</v>
-      </c>
-      <c r="O13" s="3">
-        <v>93.0</v>
-      </c>
-      <c r="P13" s="3">
-        <v>130.0</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
@@ -10430,54 +9972,22 @@
       <c r="BI13" s="3"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="B14" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="C14" s="3">
-        <v>84.0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>96.0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>29.0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>288.0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>250.0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>213.0</v>
-      </c>
-      <c r="I14" s="3">
-        <v>206.0</v>
-      </c>
-      <c r="J14" s="3">
-        <v>168.0</v>
-      </c>
-      <c r="K14" s="3">
-        <v>90.0</v>
-      </c>
-      <c r="L14" s="3">
-        <v>225.0</v>
-      </c>
-      <c r="M14" s="3">
-        <v>227.0</v>
-      </c>
-      <c r="N14" s="3">
-        <v>188.0</v>
-      </c>
-      <c r="O14" s="3">
-        <v>245.0</v>
-      </c>
-      <c r="P14" s="3">
-        <v>301.0</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
@@ -10525,54 +10035,22 @@
       <c r="BI14" s="3"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="B15" s="3">
-        <v>289.0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>58.0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>255.0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>129.0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>232.0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>227.0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>246.0</v>
-      </c>
-      <c r="I15" s="3">
-        <v>119.0</v>
-      </c>
-      <c r="J15" s="3">
-        <v>307.0</v>
-      </c>
-      <c r="K15" s="3">
-        <v>252.0</v>
-      </c>
-      <c r="L15" s="3">
-        <v>154.0</v>
-      </c>
-      <c r="M15" s="3">
-        <v>159.0</v>
-      </c>
-      <c r="N15" s="3">
-        <v>240.0</v>
-      </c>
-      <c r="O15" s="3">
-        <v>250.0</v>
-      </c>
-      <c r="P15" s="3">
-        <v>194.0</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
@@ -10620,54 +10098,22 @@
       <c r="BI15" s="3"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="B16" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="C16" s="3">
-        <v>119.0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>303.0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>114.0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>31.0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>244.0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>257.0</v>
-      </c>
-      <c r="I16" s="3">
-        <v>209.0</v>
-      </c>
-      <c r="J16" s="3">
-        <v>262.0</v>
-      </c>
-      <c r="K16" s="3">
-        <v>37.0</v>
-      </c>
-      <c r="L16" s="3">
-        <v>291.0</v>
-      </c>
-      <c r="M16" s="3">
-        <v>147.0</v>
-      </c>
-      <c r="N16" s="3">
-        <v>57.0</v>
-      </c>
-      <c r="O16" s="3">
-        <v>69.0</v>
-      </c>
-      <c r="P16" s="3">
-        <v>123.0</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
@@ -11094,7 +10540,7 @@
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="5"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -11157,7 +10603,7 @@
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="5"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -11220,7 +10666,7 @@
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="5"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -11283,7 +10729,7 @@
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -11346,7 +10792,7 @@
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="5"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -11409,7 +10855,7 @@
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="5"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -11472,7 +10918,7 @@
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="5"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -11535,7 +10981,7 @@
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="6"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -11598,7 +11044,7 @@
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="6"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -11661,7 +11107,7 @@
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="6"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>

</xml_diff>